<commit_message>
Insert 0 if azs_code not found
</commit_message>
<xml_diff>
--- a/92.xlsx
+++ b/92.xlsx
@@ -1,30 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\scrpt\agas-master\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="18015" windowHeight="8145"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8145" windowWidth="18015" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Лист1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Лист1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="152511" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="27">
   <si>
     <t>Клиент</t>
   </si>
@@ -65,6 +55,9 @@
     <t>Барнаул</t>
   </si>
   <si>
+    <t>01.04-04.06</t>
+  </si>
+  <si>
     <t>АГАС_15 сек_21.05 - 04.06.2018_32ХХХ</t>
   </si>
   <si>
@@ -102,86 +95,83 @@
   </si>
   <si>
     <t>г.Барнаул, ул.Сельскохозяйственная, 1а</t>
-  </si>
-  <si>
-    <t>01.04-04.06</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="2">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-"/>
+    <numFmt formatCode="_-* #,##0\ _₽_-;\-* #,##0\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-" numFmtId="164"/>
+    <numFmt formatCode="_-* #,##0.00\ _₽_-;\-* #,##0.00\ _₽_-;_-* &quot;-&quot;??\ _₽_-;_-@_-" numFmtId="165"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="1"/>
+      <color theme="0"/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
     <font>
-      <b/>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <b val="1"/>
+      <color theme="0"/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="204"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
     </font>
     <font>
-      <b/>
+      <name val="Times New Roman"/>
+      <charset val="204"/>
+      <family val="1"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-      <charset val="204"/>
     </font>
   </fonts>
   <fills count="7">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -309,100 +299,91 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="165"/>
   </cellStyleXfs>
-  <cellXfs count="28">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="29">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1" locked="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="4" fontId="6" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="4" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf borderId="4" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="6" fillId="5" fontId="2" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="6" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="7" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="2" fontId="5" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+      <protection hidden="1" locked="1"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="6" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="4" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="4" fillId="0" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="4" fillId="5" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" borderId="5" fillId="5" fontId="2" numFmtId="49" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection hidden="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="2" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="3" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="4" fillId="3" fontId="4" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Финансовый" xfId="1" builtinId="3"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="0"/>
+    <cellStyle builtinId="3" name="Финансовый" xfId="1"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
 </styleSheet>
 </file>
 
@@ -668,335 +649,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
   <cols>
-    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="21.140625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="21" width="20.85546875"/>
+    <col bestFit="1" customWidth="1" max="4" min="4" style="21" width="11.5703125"/>
+    <col bestFit="1" customWidth="1" max="5" min="5" style="21" width="15.7109375"/>
+    <col bestFit="1" customWidth="1" max="6" min="6" style="21" width="23.28515625"/>
+    <col bestFit="1" customWidth="1" max="7" min="7" style="21" width="30"/>
+    <col bestFit="1" customWidth="1" max="9" min="9" style="21" width="21.140625"/>
+    <col bestFit="1" customWidth="1" max="10" min="10" style="21" width="25.7109375"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-      <c r="B1" s="20" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="1" t="n"/>
+      <c r="B1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="D1" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="E1" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="F1" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="20" t="s">
+      <c r="G1" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="20" t="s">
+      <c r="H1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="22" t="s">
+      <c r="I1" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="20" t="s">
+      <c r="J1" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="23" t="s">
+      <c r="K1" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="24" t="s">
+      <c r="L1" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4" t="s">
+      <c r="P1" s="12" t="n"/>
+      <c r="Q1" s="12" t="n"/>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="1" t="n"/>
+      <c r="P2" s="12" t="n"/>
+      <c r="Q2" s="12" t="n"/>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="11" t="n"/>
+      <c r="B3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="3" t="n">
         <v>9</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="G3" s="5">
+      <c r="G3" s="3" t="n">
         <v>480</v>
       </c>
-      <c r="H3" s="5">
+      <c r="H3" s="3" t="n">
         <v>15</v>
       </c>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="n">
+        <v>15</v>
+      </c>
+      <c r="K3" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="M3" s="2" t="n"/>
+      <c r="N3" s="2" t="n"/>
+      <c r="O3" s="2" t="n"/>
+      <c r="P3" s="5" t="n"/>
+      <c r="Q3" s="11" t="n"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="11" t="n"/>
+      <c r="B4" s="11" t="n"/>
+      <c r="C4" s="11" t="n"/>
+      <c r="D4" s="11" t="n"/>
+      <c r="E4" s="11" t="n"/>
+      <c r="F4" s="11" t="n"/>
+      <c r="G4" s="11" t="n"/>
+      <c r="H4" s="11" t="n"/>
+      <c r="I4" s="11" t="n"/>
+      <c r="J4" s="11" t="n"/>
+      <c r="K4" s="11" t="n"/>
+      <c r="L4" s="11" t="n"/>
+      <c r="M4" s="11" t="n"/>
+      <c r="N4" s="11" t="n"/>
+      <c r="O4" s="11" t="n"/>
+      <c r="P4" s="11" t="n"/>
+      <c r="Q4" s="11" t="n"/>
+    </row>
+    <row customHeight="1" ht="60" r="5" s="21" spans="1:17">
+      <c r="A5" s="11" t="n"/>
+      <c r="B5" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" s="24" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="Q5" s="6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="11" t="n"/>
+      <c r="B6" s="7" t="n">
+        <v>10001</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="I6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="M6" s="20" t="n">
+        <v>960</v>
+      </c>
+      <c r="P6" s="8" t="n">
+        <v>182282</v>
+      </c>
+      <c r="Q6" s="9">
+        <f>P6-M6</f>
+        <v/>
+      </c>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="11" t="n"/>
+      <c r="B7" s="7" t="n">
+        <v>10006</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="J3" s="5">
-        <v>15</v>
-      </c>
-      <c r="K3" s="6">
-        <v>32</v>
-      </c>
-      <c r="L3" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="7"/>
-      <c r="Q3" s="3"/>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="L4" s="3"/>
-      <c r="M4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="O4" s="3"/>
-      <c r="P4" s="3"/>
-      <c r="Q4" s="3"/>
-    </row>
-    <row r="5" spans="1:17" ht="60" x14ac:dyDescent="0.25">
-      <c r="A5" s="3"/>
-      <c r="B5" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="E5" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="18"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="17" t="s">
-        <v>17</v>
-      </c>
-      <c r="J5" s="18"/>
-      <c r="K5" s="18"/>
-      <c r="L5" s="18"/>
-      <c r="M5" s="19" t="s">
-        <v>18</v>
-      </c>
-      <c r="N5" s="18"/>
-      <c r="O5" s="18"/>
-      <c r="P5" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="Q5" s="10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="11">
-        <v>10001</v>
-      </c>
-      <c r="C6" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="18"/>
-      <c r="G6" s="18"/>
-      <c r="H6" s="18"/>
-      <c r="I6" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="J6" s="18"/>
-      <c r="K6" s="18"/>
-      <c r="L6" s="18"/>
-      <c r="M6" s="26">
+      <c r="M7" s="20">
+        <f>M6</f>
+        <v/>
+      </c>
+      <c r="P7" s="8" t="n">
+        <v>178238</v>
+      </c>
+      <c r="Q7" s="9">
+        <f>P7-M7</f>
+        <v/>
+      </c>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="11" t="n"/>
+      <c r="B8" s="13" t="n">
+        <v>11002</v>
+      </c>
+      <c r="C8" s="13" t="n"/>
+      <c r="D8" s="13" t="n"/>
+      <c r="E8" s="14" t="n"/>
+      <c r="I8" s="14" t="n"/>
+      <c r="M8" s="20" t="n"/>
+      <c r="N8" t="n">
         <v>960</v>
       </c>
-      <c r="N6" s="18"/>
-      <c r="O6" s="18"/>
-      <c r="P6" s="12"/>
-      <c r="Q6" s="13">
-        <f t="shared" ref="Q6:Q11" si="0">P6-M6</f>
-        <v>-960</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
-      <c r="B7" s="11">
-        <v>10006</v>
-      </c>
-      <c r="C7" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="E7" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="25" t="s">
-        <v>25</v>
-      </c>
-      <c r="J7" s="18"/>
-      <c r="K7" s="18"/>
-      <c r="L7" s="18"/>
-      <c r="M7" s="26">
-        <f t="shared" ref="M7:M11" si="1">M6</f>
+      <c r="P8" s="15" t="n">
+        <v>272919</v>
+      </c>
+      <c r="Q8" s="9" t="n"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="11" t="n"/>
+      <c r="B9" s="13" t="n">
+        <v>11003</v>
+      </c>
+      <c r="C9" s="13" t="n"/>
+      <c r="D9" s="13" t="n"/>
+      <c r="E9" s="14" t="n"/>
+      <c r="I9" s="14" t="n"/>
+      <c r="M9" s="20" t="n"/>
+      <c r="N9" t="n">
         <v>960</v>
       </c>
-      <c r="N7" s="18"/>
-      <c r="O7" s="18"/>
-      <c r="P7" s="12"/>
-      <c r="Q7" s="13">
-        <f t="shared" si="0"/>
-        <v>-960</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="14">
+      <c r="P9" s="15" t="n">
+        <v>284889</v>
+      </c>
+      <c r="Q9" s="9" t="n"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="11" t="n"/>
+      <c r="B10" s="13" t="n">
+        <v>11006</v>
+      </c>
+      <c r="C10" s="13" t="n"/>
+      <c r="D10" s="13" t="n"/>
+      <c r="E10" s="14" t="n"/>
+      <c r="I10" s="14" t="n"/>
+      <c r="M10" s="20" t="n"/>
+      <c r="N10" t="n">
+        <v>960</v>
+      </c>
+      <c r="P10" s="15" t="n">
+        <v>284994</v>
+      </c>
+      <c r="Q10" s="9" t="n"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="11" t="n"/>
+      <c r="B11" s="13" t="n">
         <v>10013</v>
       </c>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="26">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
-      <c r="P8" s="15"/>
-      <c r="Q8" s="13">
-        <f t="shared" si="0"/>
-        <v>-960</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B9" s="27">
+      <c r="C11" s="13" t="n"/>
+      <c r="D11" s="13" t="n"/>
+      <c r="E11" s="14" t="n"/>
+      <c r="F11" s="14" t="n"/>
+      <c r="G11" s="14" t="n"/>
+      <c r="H11" s="14" t="n"/>
+      <c r="I11" s="14" t="n"/>
+      <c r="J11" s="14" t="n"/>
+      <c r="K11" s="14" t="n"/>
+      <c r="L11" s="14" t="n"/>
+      <c r="M11" s="20">
+        <f>M7</f>
+        <v/>
+      </c>
+      <c r="P11" s="14" t="n">
+        <v>190020</v>
+      </c>
+      <c r="Q11" s="9">
+        <f>P11-M11</f>
+        <v/>
+      </c>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="B12" s="13" t="n">
         <v>10017</v>
       </c>
-      <c r="M9" s="26">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-      <c r="N9" s="18"/>
-      <c r="O9" s="18"/>
-      <c r="Q9" s="13">
-        <f t="shared" si="0"/>
-        <v>-960</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B10" s="27">
+      <c r="M12" s="20">
+        <f>M11</f>
+        <v/>
+      </c>
+      <c r="P12" t="n">
+        <v>190016</v>
+      </c>
+      <c r="Q12" s="9">
+        <f>P12-M12</f>
+        <v/>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="B13" s="13" t="n">
         <v>10047</v>
       </c>
-      <c r="M10" s="26">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-      <c r="N10" s="18"/>
-      <c r="O10" s="18"/>
-      <c r="Q10" s="13">
-        <f t="shared" si="0"/>
-        <v>-960</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="M11" s="26">
-        <f t="shared" si="1"/>
-        <v>960</v>
-      </c>
-      <c r="N11" s="18"/>
-      <c r="O11" s="18"/>
-      <c r="Q11" s="13">
-        <f t="shared" si="0"/>
-        <v>-960</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="Q12" s="16">
-        <f>SUM(Q6:Q11)</f>
-        <v>-5760</v>
+      <c r="M13" s="20">
+        <f>M12</f>
+        <v/>
+      </c>
+      <c r="P13" t="n">
+        <v>186642</v>
+      </c>
+      <c r="Q13" s="9">
+        <f>P13-M13</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="M14" s="20">
+        <f>M13</f>
+        <v/>
+      </c>
+      <c r="Q14" s="9">
+        <f>P14-M14</f>
+        <v/>
+      </c>
+    </row>
+    <row customHeight="1" ht="15.75" r="15" s="21" spans="1:17">
+      <c r="Q15" s="10">
+        <f>SUM(Q6:Q14)</f>
+        <v/>
       </c>
     </row>
   </sheetData>
   <mergeCells count="24">
-    <mergeCell ref="M8:O8"/>
-    <mergeCell ref="M9:O9"/>
-    <mergeCell ref="M10:O10"/>
-    <mergeCell ref="M11:O11"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="I6:L6"/>
-    <mergeCell ref="M6:O6"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="I7:L7"/>
-    <mergeCell ref="M7:O7"/>
     <mergeCell ref="E5:H5"/>
     <mergeCell ref="I5:L5"/>
     <mergeCell ref="M5:O5"/>
@@ -1011,7 +1003,17 @@
     <mergeCell ref="J1:J2"/>
     <mergeCell ref="K1:K2"/>
     <mergeCell ref="L1:O2"/>
+    <mergeCell ref="M11:O11"/>
+    <mergeCell ref="M12:O12"/>
+    <mergeCell ref="M13:O13"/>
+    <mergeCell ref="M14:O14"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="I6:L6"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="I7:L7"/>
+    <mergeCell ref="M7:O7"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add possibility using multiple reports
</commit_message>
<xml_diff>
--- a/92.xlsx
+++ b/92.xlsx
@@ -822,7 +822,7 @@
         <v>960</v>
       </c>
       <c r="P6" s="8" t="n">
-        <v>182282</v>
+        <v>274250</v>
       </c>
       <c r="Q6" s="9">
         <f>P6-M6</f>
@@ -851,7 +851,7 @@
         <v/>
       </c>
       <c r="P7" s="8" t="n">
-        <v>178238</v>
+        <v>110388</v>
       </c>
       <c r="Q7" s="9">
         <f>P7-M7</f>
@@ -872,7 +872,7 @@
         <v>960</v>
       </c>
       <c r="P8" s="15" t="n">
-        <v>272919</v>
+        <v>303090</v>
       </c>
       <c r="Q8" s="9" t="n"/>
     </row>
@@ -890,7 +890,7 @@
         <v>960</v>
       </c>
       <c r="P9" s="15" t="n">
-        <v>284889</v>
+        <v>310986</v>
       </c>
       <c r="Q9" s="9" t="n"/>
     </row>
@@ -908,7 +908,7 @@
         <v>960</v>
       </c>
       <c r="P10" s="15" t="n">
-        <v>284994</v>
+        <v>311727</v>
       </c>
       <c r="Q10" s="9" t="n"/>
     </row>
@@ -932,7 +932,7 @@
         <v/>
       </c>
       <c r="P11" s="14" t="n">
-        <v>190020</v>
+        <v>284604</v>
       </c>
       <c r="Q11" s="9">
         <f>P11-M11</f>
@@ -948,7 +948,7 @@
         <v/>
       </c>
       <c r="P12" t="n">
-        <v>190016</v>
+        <v>441228</v>
       </c>
       <c r="Q12" s="9">
         <f>P12-M12</f>
@@ -964,7 +964,7 @@
         <v/>
       </c>
       <c r="P13" t="n">
-        <v>186642</v>
+        <v>282884</v>
       </c>
       <c r="Q13" s="9">
         <f>P13-M13</f>

</xml_diff>